<commit_message>
connected app.py to upload.js, display spreadsheet when completed
</commit_message>
<xml_diff>
--- a/backend/template.xlsx
+++ b/backend/template.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
   <si>
     <t>SALES ORDER</t>
   </si>
@@ -74,6 +74,34 @@
   </si>
   <si>
     <t>Cases</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>8/64 oz Suntropics Mango Nectar</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>8/64 oz Suntropics Guava Nectar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8/64 oz  Suntropics Calamansi - </t>
+  </si>
+  <si>
+    <t>8/64 oz  Suntropics Passion OJ Guava 100% Juice</t>
   </si>
   <si>
     <t>CODING INSTRUCTIONS:</t>
@@ -114,7 +142,7 @@
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="&quot; &quot;&quot;$&quot;* #,##0.00&quot; &quot;;&quot; &quot;&quot;$&quot;* (#,##0.00);&quot; &quot;&quot;$&quot;* &quot;-&quot;??&quot; &quot;"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -171,13 +199,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="1"/>
-      <sz val="12"/>
-      <color indexed="11"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color indexed="11"/>
       <name val="Arial"/>
@@ -207,11 +228,11 @@
     <font>
       <b val="1"/>
       <sz val="10"/>
-      <color indexed="14"/>
+      <color indexed="13"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -224,14 +245,8 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="16">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -296,76 +311,6 @@
       </top>
       <bottom style="medium">
         <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -418,6 +363,36 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -511,28 +486,16 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -547,10 +510,10 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -566,6 +529,18 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="59" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="59" fontId="5" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -574,13 +549,13 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="2" fontId="6" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="6" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="6" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="59" fontId="6" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -589,7 +564,7 @@
     <xf numFmtId="2" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -598,43 +573,43 @@
     <xf numFmtId="49" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="2" fontId="13" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="15" fontId="14" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="15" fontId="13" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -661,7 +636,6 @@
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffdd0806"/>
       <rgbColor rgb="ff0000d4"/>
-      <rgbColor rgb="ffffff00"/>
       <rgbColor rgb="ff808080"/>
     </indexedColors>
   </colors>
@@ -681,7 +655,7 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>743396</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>67499</xdr:rowOff>
+      <xdr:rowOff>67498</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -700,7 +674,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="86990" y="57598"/>
+          <a:off x="86990" y="57597"/>
           <a:ext cx="2332807" cy="1076702"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2032,11 +2006,11 @@
         <v>10</v>
       </c>
       <c r="C20" s="9"/>
-      <c r="D20" s="21"/>
-      <c r="E20" t="s" s="22">
-        <v>2</v>
-      </c>
-      <c r="F20" s="23"/>
+      <c r="D20" s="7"/>
+      <c r="E20" t="s" s="15">
+        <v>2</v>
+      </c>
+      <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
@@ -2049,7 +2023,7 @@
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="7"/>
-      <c r="E21" t="s" s="24">
+      <c r="E21" t="s" s="15">
         <v>2</v>
       </c>
       <c r="F21" s="7"/>
@@ -2065,7 +2039,7 @@
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
-      <c r="E22" t="s" s="24">
+      <c r="E22" t="s" s="15">
         <v>2</v>
       </c>
       <c r="F22" s="7"/>
@@ -2081,7 +2055,7 @@
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="7"/>
-      <c r="E23" t="s" s="25">
+      <c r="E23" t="s" s="15">
         <v>2</v>
       </c>
       <c r="F23" s="7"/>
@@ -2092,10 +2066,10 @@
     </row>
     <row r="24" ht="16.5" customHeight="1">
       <c r="A24" s="16"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
       <c r="D24" s="16"/>
-      <c r="E24" t="s" s="14">
+      <c r="E24" t="s" s="22">
         <v>14</v>
       </c>
       <c r="F24" s="16"/>
@@ -2105,24 +2079,24 @@
       <c r="J24" s="2"/>
     </row>
     <row r="25" ht="16.5" customHeight="1">
-      <c r="A25" t="s" s="27">
+      <c r="A25" t="s" s="23">
         <v>15</v>
       </c>
-      <c r="B25" s="28"/>
-      <c r="C25" t="s" s="29">
+      <c r="B25" s="24"/>
+      <c r="C25" t="s" s="25">
         <v>16</v>
       </c>
-      <c r="D25" t="s" s="30">
+      <c r="D25" t="s" s="26">
         <v>17</v>
       </c>
-      <c r="E25" s="31"/>
-      <c r="F25" t="s" s="30">
+      <c r="E25" s="27"/>
+      <c r="F25" t="s" s="26">
         <v>18</v>
       </c>
-      <c r="G25" t="s" s="32">
+      <c r="G25" t="s" s="28">
         <v>19</v>
       </c>
-      <c r="H25" s="33"/>
+      <c r="H25" s="29"/>
       <c r="I25" s="13"/>
       <c r="J25" s="2"/>
     </row>
@@ -2130,16 +2104,16 @@
       <c r="A26" t="s" s="10">
         <v>2</v>
       </c>
-      <c r="B26" t="s" s="34">
+      <c r="B26" t="s" s="30">
         <v>20</v>
       </c>
       <c r="C26" t="s" s="10">
         <v>2</v>
       </c>
-      <c r="D26" t="s" s="10">
-        <v>2</v>
-      </c>
-      <c r="E26" s="35"/>
+      <c r="D26" t="s" s="22">
+        <v>21</v>
+      </c>
+      <c r="E26" s="31"/>
       <c r="F26" t="s" s="10">
         <v>2</v>
       </c>
@@ -2151,20 +2125,20 @@
       <c r="J26" s="2"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" t="s" s="36">
-        <v>2</v>
-      </c>
-      <c r="B27" t="s" s="37">
+      <c r="A27" t="s" s="32">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s" s="33">
         <v>20</v>
       </c>
-      <c r="C27" t="s" s="36">
-        <v>2</v>
-      </c>
-      <c r="D27" t="s" s="36">
-        <v>2</v>
-      </c>
-      <c r="E27" s="38"/>
-      <c r="F27" t="s" s="36">
+      <c r="C27" t="s" s="32">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s" s="22">
+        <v>22</v>
+      </c>
+      <c r="E27" s="34"/>
+      <c r="F27" t="s" s="32">
         <v>2</v>
       </c>
       <c r="G27" t="s" s="10">
@@ -2175,23 +2149,23 @@
       <c r="J27" s="2"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" t="s" s="36">
-        <v>2</v>
-      </c>
-      <c r="B28" t="s" s="37">
+      <c r="A28" t="s" s="32">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s" s="33">
         <v>20</v>
       </c>
-      <c r="C28" t="s" s="36">
-        <v>2</v>
-      </c>
-      <c r="D28" t="s" s="36">
-        <v>2</v>
-      </c>
-      <c r="E28" s="38"/>
-      <c r="F28" t="s" s="36">
-        <v>2</v>
-      </c>
-      <c r="G28" t="s" s="36">
+      <c r="C28" t="s" s="32">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s" s="22">
+        <v>23</v>
+      </c>
+      <c r="E28" s="34"/>
+      <c r="F28" t="s" s="32">
+        <v>2</v>
+      </c>
+      <c r="G28" t="s" s="32">
         <v>2</v>
       </c>
       <c r="H28" s="13"/>
@@ -2199,23 +2173,23 @@
       <c r="J28" s="2"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" t="s" s="36">
-        <v>2</v>
-      </c>
-      <c r="B29" t="s" s="37">
+      <c r="A29" t="s" s="32">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s" s="33">
         <v>20</v>
       </c>
-      <c r="C29" t="s" s="36">
+      <c r="C29" t="s" s="35">
         <v>2</v>
       </c>
       <c r="D29" t="s" s="36">
-        <v>2</v>
-      </c>
-      <c r="E29" s="38"/>
-      <c r="F29" t="s" s="36">
-        <v>2</v>
-      </c>
-      <c r="G29" t="s" s="36">
+        <v>24</v>
+      </c>
+      <c r="E29" s="37"/>
+      <c r="F29" t="s" s="32">
+        <v>2</v>
+      </c>
+      <c r="G29" t="s" s="32">
         <v>2</v>
       </c>
       <c r="H29" s="13"/>
@@ -2223,14 +2197,14 @@
       <c r="J29" s="2"/>
     </row>
     <row r="30" ht="16.5" customHeight="1">
-      <c r="A30" t="s" s="36">
-        <v>2</v>
-      </c>
-      <c r="B30" t="s" s="37">
+      <c r="A30" t="s" s="32">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s" s="33">
         <v>20</v>
       </c>
       <c r="C30" s="7"/>
-      <c r="D30" s="9"/>
+      <c r="D30" s="38"/>
       <c r="E30" t="s" s="39">
         <v>19</v>
       </c>
@@ -2256,13 +2230,13 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" t="s" s="8">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
       <c r="E32" t="s" s="12">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F32" s="40"/>
       <c r="G32" s="44"/>
@@ -2283,8 +2257,8 @@
       <c r="J33" s="2"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" t="s" s="36">
-        <v>23</v>
+      <c r="A34" t="s" s="32">
+        <v>27</v>
       </c>
       <c r="B34" s="46"/>
       <c r="C34" s="46"/>
@@ -2321,14 +2295,14 @@
       <c r="J36" s="2"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" t="s" s="37">
-        <v>24</v>
+      <c r="A37" t="s" s="33">
+        <v>28</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" t="s" s="47">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F37" s="40"/>
       <c r="G37" s="44"/>
@@ -2342,7 +2316,7 @@
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
       <c r="E38" t="s" s="48">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F38" s="9"/>
       <c r="G38" s="7"/>
@@ -2355,7 +2329,7 @@
       <c r="B39" s="49"/>
       <c r="C39" s="49"/>
       <c r="D39" t="s" s="50">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E39" s="51"/>
       <c r="F39" s="51"/>
@@ -2368,7 +2342,7 @@
       <c r="A40" s="49"/>
       <c r="B40" s="53"/>
       <c r="C40" t="s" s="50">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D40" s="54"/>
       <c r="E40" s="54"/>
@@ -2381,7 +2355,7 @@
     <row r="41" ht="31.5" customHeight="1">
       <c r="A41" s="7"/>
       <c r="B41" t="s" s="55">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C41" s="56"/>
       <c r="D41" s="56"/>
@@ -2410,7 +2384,7 @@
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" t="s" s="58">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>

</xml_diff>